<commit_message>
Add GD tinypico BOM + POS files
</commit_message>
<xml_diff>
--- a/tinypico-goodisplay/production/POS.xlsx
+++ b/tinypico-goodisplay/production/POS.xlsx
@@ -112,7 +112,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1:E1"/>
@@ -257,7 +257,7 @@
         <v>111.95</v>
       </c>
       <c r="C7" s="3">
-        <v>-46.5625</v>
+        <v>-46.549999999999997</v>
       </c>
       <c r="D7" s="3">
         <v>90</v>
@@ -383,17 +383,17 @@
     <row r="14" spans="1:5">
       <c r="A14" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>C13</t>
         </is>
       </c>
       <c r="B14" s="3">
-        <v>82.700000000000003</v>
+        <v>116.2</v>
       </c>
       <c r="C14" s="3">
-        <v>-43.950000000000003</v>
+        <v>-50.549999999999997</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -402,17 +402,17 @@
     <row r="15" spans="1:5">
       <c r="A15" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>C14</t>
         </is>
       </c>
       <c r="B15" s="3">
-        <v>82.700000000000003</v>
+        <v>122.8</v>
       </c>
       <c r="C15" s="3">
-        <v>-46.350000000000001</v>
+        <v>-50.549999999999997</v>
       </c>
       <c r="D15" s="3">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -421,17 +421,17 @@
     <row r="16" spans="1:5">
       <c r="A16" t="inlineStr">
         <is>
-          <t>D3</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="B16" s="3">
         <v>82.700000000000003</v>
       </c>
       <c r="C16" s="3">
-        <v>-41.549999999999997</v>
+        <v>-43.950000000000003</v>
       </c>
       <c r="D16" s="3">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -440,14 +440,14 @@
     <row r="17" spans="1:5">
       <c r="A17" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="B17" s="3">
-        <v>97.599999999999994</v>
+        <v>82.700000000000003</v>
       </c>
       <c r="C17" s="3">
-        <v>-39.004398999999999</v>
+        <v>-46.350000000000001</v>
       </c>
       <c r="D17" s="3">
         <v>180</v>
@@ -459,17 +459,17 @@
     <row r="18" spans="1:5">
       <c r="A18" t="inlineStr">
         <is>
-          <t>JP1</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="B18" s="3">
-        <v>107.19</v>
+        <v>82.700000000000003</v>
       </c>
       <c r="C18" s="3">
-        <v>-50.740000000000002</v>
+        <v>-41.549999999999997</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
@@ -478,17 +478,17 @@
     <row r="19" spans="1:5">
       <c r="A19" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>D4</t>
         </is>
       </c>
       <c r="B19" s="3">
-        <v>77.549999999999997</v>
+        <v>116.8</v>
       </c>
       <c r="C19" s="3">
-        <v>-45.049999999999997</v>
+        <v>-36.994999999999997</v>
       </c>
       <c r="D19" s="3">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -497,17 +497,17 @@
     <row r="20" spans="1:5">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>D5</t>
         </is>
       </c>
       <c r="B20" s="3">
-        <v>91.200000000000003</v>
+        <v>120.34999999999999</v>
       </c>
       <c r="C20" s="3">
-        <v>-47.200000000000003</v>
+        <v>-37.049999999999997</v>
       </c>
       <c r="D20" s="3">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -516,14 +516,14 @@
     <row r="21" spans="1:5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B21" s="3">
-        <v>88</v>
+        <v>97.599999999999994</v>
       </c>
       <c r="C21" s="3">
-        <v>-47.549999999999997</v>
+        <v>-39.004398999999999</v>
       </c>
       <c r="D21" s="3">
         <v>180</v>
@@ -535,17 +535,17 @@
     <row r="22" spans="1:5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>JP1</t>
         </is>
       </c>
       <c r="B22" s="3">
-        <v>100.7</v>
+        <v>107.19</v>
       </c>
       <c r="C22" s="3">
-        <v>-50.75</v>
+        <v>-50.740000000000002</v>
       </c>
       <c r="D22" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -554,19 +554,190 @@
     <row r="23" spans="1:5">
       <c r="A23" t="inlineStr">
         <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="B23" s="3">
+        <v>77.549999999999997</v>
+      </c>
+      <c r="C23" s="3">
+        <v>-45.049999999999997</v>
+      </c>
+      <c r="D23" s="3">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Q1</t>
+        </is>
+      </c>
+      <c r="B24" s="3">
+        <v>91.200000000000003</v>
+      </c>
+      <c r="C24" s="3">
+        <v>-47.200000000000003</v>
+      </c>
+      <c r="D24" s="3">
+        <v>-90</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>R1</t>
+        </is>
+      </c>
+      <c r="B25" s="3">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3">
+        <v>-47.549999999999997</v>
+      </c>
+      <c r="D25" s="3">
+        <v>180</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="B26" s="3">
+        <v>100.7</v>
+      </c>
+      <c r="C26" s="3">
+        <v>-50.75</v>
+      </c>
+      <c r="D26" s="3">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>R3</t>
         </is>
       </c>
-      <c r="B23" s="3">
+      <c r="B27" s="3">
         <v>113.25</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C27" s="3">
         <v>-50.600000000000001</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D27" s="3">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>R5</t>
+        </is>
+      </c>
+      <c r="B28" s="3">
+        <v>115.95</v>
+      </c>
+      <c r="C28" s="3">
+        <v>-45.350000000000001</v>
+      </c>
+      <c r="D28" s="3">
+        <v>90</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="B29" s="3">
+        <v>123.65000000000001</v>
+      </c>
+      <c r="C29" s="3">
+        <v>-41.475000000000001</v>
+      </c>
+      <c r="D29" s="3">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>R7</t>
+        </is>
+      </c>
+      <c r="B30" s="3">
+        <v>123.3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>-37.424999999999997</v>
+      </c>
+      <c r="D30" s="3">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>U2</t>
+        </is>
+      </c>
+      <c r="B31" s="3">
+        <v>119.95</v>
+      </c>
+      <c r="C31" s="3">
+        <v>-43.649999999999999</v>
+      </c>
+      <c r="D31" s="3">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Y1</t>
+        </is>
+      </c>
+      <c r="B32" s="3">
+        <v>119.5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>-50.950000000000003</v>
+      </c>
+      <c r="D32" s="3">
+        <v>180</v>
+      </c>
+      <c r="E32" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>